<commit_message>
[REQEUST FORM][Create New Request] Added: 3114 Send Email Notification - Critical Parts
</commit_message>
<xml_diff>
--- a/storage/formatStorage/Excel_format.xlsx
+++ b/storage/formatStorage/Excel_format.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sorisantos.r21\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\hinsei\server\storage\formatStorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CA3043-7226-40DD-9873-D16756755A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE69C76-DFC3-4DEC-81D7-049EDA4FF8C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19024,10 +19024,10 @@
   <dimension ref="B4:AB21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="13" ySplit="9" topLeftCell="Q10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="13" ySplit="9" topLeftCell="S10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
+      <selection pane="bottomRight" activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19271,9 +19271,7 @@
       <c r="S10" s="9"/>
       <c r="T10" s="9"/>
       <c r="U10" s="9"/>
-      <c r="V10" s="9">
-        <v>121</v>
-      </c>
+      <c r="V10" s="9"/>
       <c r="W10" s="9"/>
       <c r="X10" s="9"/>
       <c r="Y10" s="15"/>

</xml_diff>